<commit_message>
Automatic commit: Move 'spa-create-automation' from QA to Production
</commit_message>
<xml_diff>
--- a/tutorials/spa-create-automation/Orders.xlsx
+++ b/tutorials/spa-create-automation/Orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/celine_audin_sap_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE868B5-6BDD-49DE-89CD-0D1D9BEDB2D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A58B570E-2253-439A-B0F5-F1D7DBA3E3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B8B3745C-EC5C-4B29-9CCB-5F42CEDDE2C3}"/>
+    <workbookView xWindow="5436" yWindow="2712" windowWidth="17280" windowHeight="10074" xr2:uid="{EC4734C5-5DFC-4B51-805F-38417827CDCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,82 +34,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Order Number</t>
   </si>
   <si>
+    <t>Order Amount</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Shipping Country</t>
+  </si>
+  <si>
+    <t>Expected Delivery Date</t>
+  </si>
+  <si>
     <t>Order Status</t>
   </si>
   <si>
-    <t>Order Date</t>
-  </si>
-  <si>
-    <t>Order Amount</t>
-  </si>
-  <si>
-    <t>Shipping Country</t>
-  </si>
-  <si>
-    <t>Expected Delivery Date</t>
-  </si>
-  <si>
-    <t>Order 7991</t>
-  </si>
-  <si>
-    <t>Order 7918</t>
-  </si>
-  <si>
-    <t>Order 7375</t>
-  </si>
-  <si>
-    <t>Order 7311</t>
-  </si>
-  <si>
-    <t>Order 6858</t>
-  </si>
-  <si>
-    <t>Order 6368</t>
-  </si>
-  <si>
-    <t>Order 6189</t>
-  </si>
-  <si>
-    <t>Order 3115</t>
-  </si>
-  <si>
-    <t>Order 2686</t>
-  </si>
-  <si>
-    <t>Order 828</t>
+    <t>PO7991</t>
   </si>
   <si>
     <t>United States of America</t>
   </si>
   <si>
+    <t>In Time</t>
+  </si>
+  <si>
+    <t>PO7918</t>
+  </si>
+  <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>Deutchland</t>
-  </si>
-  <si>
-    <t>United staes of America</t>
-  </si>
-  <si>
-    <t>In time</t>
-  </si>
-  <si>
     <t>Urgent</t>
   </si>
   <si>
-    <t>Too late</t>
+    <t>PO7375</t>
+  </si>
+  <si>
+    <t>PO7311</t>
+  </si>
+  <si>
+    <t>PO6858</t>
+  </si>
+  <si>
+    <t>PO6368</t>
+  </si>
+  <si>
+    <t>PO6189</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>PO3115</t>
+  </si>
+  <si>
+    <t>PO2686</t>
+  </si>
+  <si>
+    <t>PO8282</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,15 +112,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,7 +136,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,12 +180,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,245 +510,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC32E5C-A1B0-44E9-A9A5-439EF67654C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593BC366-93B3-49AC-9533-B033CBC6DB6E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.41796875" customWidth="1"/>
+    <col min="5" max="5" width="17.62890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>410418.22</v>
       </c>
-      <c r="C2" s="3">
-        <v>42695</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>44582</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44590</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
+        <v>150935.13</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44583</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
+        <v>44588</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>313977.82</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44584</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44612</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>755055.4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44585</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44650</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>429358.4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44586</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44612</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43739.82</v>
+      </c>
+      <c r="C7" s="4">
+        <v>44587</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44645</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3">
-        <v>42703</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="B8" s="1">
+        <v>483574.12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44588</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44597</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3">
+        <v>273993.56</v>
+      </c>
+      <c r="C9" s="4">
+        <v>44589</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4">
+        <v>44630</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>220887.56</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44590</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2">
+        <v>44625</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B11" s="3">
+        <v>436955.64</v>
+      </c>
+      <c r="C11" s="4">
+        <v>44591</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>150935.13</v>
-      </c>
-      <c r="C3" s="3">
-        <v>42631</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3">
-        <v>42640</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>313977.81999999902</v>
-      </c>
-      <c r="C4" s="3">
-        <v>42649</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3">
-        <v>42663</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4">
-        <v>755055.4</v>
-      </c>
-      <c r="C5" s="3">
-        <v>42695</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3">
-        <v>42704</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4">
-        <v>429358.4</v>
-      </c>
-      <c r="C6" s="3">
-        <v>42687</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3">
-        <v>42694</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4">
-        <v>43739.819999999898</v>
-      </c>
-      <c r="C7" s="3">
-        <v>42687</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3">
-        <v>42699</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4">
-        <v>483574.12</v>
-      </c>
-      <c r="C8" s="3">
-        <v>42702</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3">
-        <v>42709</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4">
-        <v>273993.56</v>
-      </c>
-      <c r="C9" s="3">
-        <v>42708</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3">
-        <v>42714</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4">
-        <v>220887.56</v>
-      </c>
-      <c r="C10" s="3">
-        <v>42670</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="3">
-        <v>42679</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="4">
-        <v>436955.64</v>
-      </c>
-      <c r="C11" s="3">
-        <v>42695</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="3">
-        <v>42704</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>20</v>
+      <c r="E11" s="4">
+        <v>44650</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2nd mission with Vertical layout
</commit_message>
<xml_diff>
--- a/tutorials/spa-create-automation/Orders.xlsx
+++ b/tutorials/spa-create-automation/Orders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\sap-build-process-automation-Contribution\tutorials\spa-create-automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/celine_audin_sap_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666832F0-C3DC-49ED-8CD4-5FC3395FA0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A58B570E-2253-439A-B0F5-F1D7DBA3E3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC4734C5-5DFC-4B51-805F-38417827CDCB}"/>
+    <workbookView xWindow="5436" yWindow="2712" windowWidth="17280" windowHeight="10074" xr2:uid="{EC4734C5-5DFC-4B51-805F-38417827CDCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Order Number</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>PO8282</t>
-  </si>
-  <si>
-    <t>India</t>
   </si>
 </sst>
 </file>
@@ -517,20 +514,20 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.20703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.41796875" customWidth="1"/>
+    <col min="5" max="5" width="17.62890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -550,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -570,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -590,7 +587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -610,7 +607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -630,7 +627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -650,7 +647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="25.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -661,7 +658,7 @@
         <v>44587</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4">
         <v>44645</v>
@@ -670,7 +667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -690,7 +687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -710,7 +707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -730,7 +727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="38.700000000000003" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>